<commit_message>
paso á api so os datos que quero enviar,teño que comprobar se os envio
</commit_message>
<xml_diff>
--- a/BACK.xlsx
+++ b/BACK.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="18915" windowHeight="6720" tabRatio="480" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="18915" windowHeight="6720" tabRatio="480" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
     <sheet name="End-points" sheetId="5" r:id="rId2"/>
     <sheet name="Relación con Front - RUTAS URL" sheetId="6" r:id="rId3"/>
     <sheet name="helpers_y_middlwares" sheetId="7" r:id="rId4"/>
+    <sheet name="helpers - SQL" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'End-points'!$E$5:$M$21</definedName>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="169">
   <si>
     <t>End-point</t>
   </si>
@@ -780,6 +781,9 @@
   </si>
   <si>
     <t>Nº</t>
+  </si>
+  <si>
+    <t>listarDatos</t>
   </si>
 </sst>
 </file>
@@ -1291,6 +1295,9 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1340,9 +1347,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1678,11 +1682,11 @@
     </row>
     <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F7" s="2"/>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -1722,7 +1726,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="67" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3"/>
@@ -1754,7 +1758,7 @@
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C10" s="66"/>
+      <c r="C10" s="67"/>
       <c r="D10" s="3"/>
       <c r="E10" s="8" t="s">
         <v>47</v>
@@ -1784,7 +1788,7 @@
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C11" s="66"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="3" t="s">
         <v>63</v>
       </c>
@@ -1817,7 +1821,7 @@
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="20"/>
-      <c r="D12" s="65" t="s">
+      <c r="D12" s="66" t="s">
         <v>64</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1850,7 +1854,7 @@
       <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="65"/>
+      <c r="D13" s="66"/>
       <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1884,7 +1888,7 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="22"/>
-      <c r="D14" s="65"/>
+      <c r="D14" s="66"/>
       <c r="E14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1914,10 +1918,10 @@
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="65" t="s">
+      <c r="D15" s="66" t="s">
         <v>64</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1949,8 +1953,8 @@
     <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="65"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="66"/>
       <c r="E16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1980,10 +1984,10 @@
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D17" s="60" t="s">
         <v>64</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -2015,8 +2019,8 @@
     <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="60"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="61"/>
       <c r="E18" s="12" t="s">
         <v>14</v>
       </c>
@@ -2110,7 +2114,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="62" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="12" t="s">
@@ -2143,7 +2147,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C22" s="62"/>
+      <c r="C22" s="63"/>
       <c r="D22" s="4" t="s">
         <v>64</v>
       </c>
@@ -2174,7 +2178,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C23" s="63"/>
+      <c r="C23" s="64"/>
       <c r="D23" s="4" t="s">
         <v>64</v>
       </c>
@@ -2236,14 +2240,14 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="64"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="65"/>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J27" s="11"/>
@@ -2329,7 +2333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -3122,7 +3126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:X26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -3152,10 +3156,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="70"/>
+      <c r="G1" s="71"/>
     </row>
     <row r="2" spans="4:24" x14ac:dyDescent="0.25">
       <c r="F2" s="54" t="s">
@@ -3202,31 +3206,31 @@
       <c r="E8" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="72" t="s">
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="73" t="s">
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="S8" s="73"/>
-      <c r="T8" s="73"/>
-      <c r="U8" s="73"/>
-      <c r="V8" s="73"/>
-      <c r="W8" s="73"/>
-      <c r="X8" s="73"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="74"/>
     </row>
     <row r="9" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D9" s="55"/>
@@ -3298,29 +3302,29 @@
       <c r="E10" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74" t="s">
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74" t="s">
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
-      <c r="S10" s="74"/>
-      <c r="T10" s="74"/>
-      <c r="U10" s="74"/>
-      <c r="V10" s="74"/>
-      <c r="W10" s="74"/>
-      <c r="X10" s="74"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
     </row>
     <row r="11" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D11" s="55">
@@ -3329,29 +3333,29 @@
       <c r="E11" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74" t="s">
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="74"/>
-      <c r="P11" s="74"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="74"/>
-      <c r="T11" s="74"/>
-      <c r="U11" s="74"/>
-      <c r="V11" s="74"/>
-      <c r="W11" s="74" t="s">
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="X11" s="74"/>
+      <c r="X11" s="57"/>
     </row>
     <row r="12" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D12" s="55">
@@ -3360,29 +3364,29 @@
       <c r="E12" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74" t="s">
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="74"/>
-      <c r="T12" s="74"/>
-      <c r="U12" s="74"/>
-      <c r="V12" s="74"/>
-      <c r="W12" s="74" t="s">
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="57"/>
+      <c r="Q12" s="57"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="57"/>
+      <c r="V12" s="57"/>
+      <c r="W12" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="X12" s="74"/>
+      <c r="X12" s="57"/>
     </row>
     <row r="13" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D13" s="55">
@@ -3391,25 +3395,25 @@
       <c r="E13" s="56" t="s">
         <v>150</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="74"/>
-      <c r="N13" s="74"/>
-      <c r="O13" s="74"/>
-      <c r="P13" s="74"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="74"/>
-      <c r="S13" s="74"/>
-      <c r="T13" s="74"/>
-      <c r="U13" s="74"/>
-      <c r="V13" s="74"/>
-      <c r="W13" s="74"/>
-      <c r="X13" s="74"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="57"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
     </row>
     <row r="14" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D14" s="55">
@@ -3418,31 +3422,31 @@
       <c r="E14" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74" t="s">
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="M14" s="74"/>
-      <c r="N14" s="74"/>
-      <c r="O14" s="74"/>
-      <c r="P14" s="74" t="s">
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="74" t="s">
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="T14" s="74"/>
-      <c r="U14" s="74"/>
-      <c r="V14" s="74"/>
-      <c r="W14" s="74"/>
-      <c r="X14" s="74"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
     </row>
     <row r="15" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D15" s="55">
@@ -3451,27 +3455,27 @@
       <c r="E15" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="74"/>
-      <c r="N15" s="74"/>
-      <c r="O15" s="74"/>
-      <c r="P15" s="74"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74" t="s">
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="S15" s="74"/>
-      <c r="T15" s="74"/>
-      <c r="U15" s="74"/>
-      <c r="V15" s="74"/>
-      <c r="W15" s="74"/>
-      <c r="X15" s="74"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="57"/>
+      <c r="V15" s="57"/>
+      <c r="W15" s="57"/>
+      <c r="X15" s="57"/>
     </row>
     <row r="16" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D16" s="55">
@@ -3480,27 +3484,27 @@
       <c r="E16" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="74"/>
-      <c r="M16" s="74"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74" t="s">
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="S16" s="74"/>
-      <c r="T16" s="74"/>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74"/>
-      <c r="X16" s="74"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
     </row>
     <row r="17" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D17" s="55">
@@ -3509,27 +3513,27 @@
       <c r="E17" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74" t="s">
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="S17" s="74"/>
-      <c r="T17" s="74"/>
-      <c r="U17" s="74"/>
-      <c r="V17" s="74"/>
-      <c r="W17" s="74"/>
-      <c r="X17" s="74"/>
+      <c r="S17" s="57"/>
+      <c r="T17" s="57"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
     </row>
     <row r="18" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D18" s="55">
@@ -3538,27 +3542,27 @@
       <c r="E18" s="56" t="s">
         <v>155</v>
       </c>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="N18" s="74"/>
-      <c r="O18" s="74"/>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74" t="s">
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="S18" s="74"/>
-      <c r="T18" s="74"/>
-      <c r="U18" s="74"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="74"/>
-      <c r="X18" s="74"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="57"/>
+      <c r="V18" s="57"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
     </row>
     <row r="19" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D19" s="55">
@@ -3567,27 +3571,27 @@
       <c r="E19" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="74"/>
-      <c r="N19" s="74"/>
-      <c r="O19" s="74"/>
-      <c r="P19" s="74"/>
-      <c r="Q19" s="74"/>
-      <c r="R19" s="74" t="s">
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="57"/>
+      <c r="R19" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="S19" s="74"/>
-      <c r="T19" s="74"/>
-      <c r="U19" s="74"/>
-      <c r="V19" s="74"/>
-      <c r="W19" s="74"/>
-      <c r="X19" s="74"/>
+      <c r="S19" s="57"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
     </row>
     <row r="20" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D20" s="55">
@@ -3596,27 +3600,27 @@
       <c r="E20" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="74" t="s">
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="S20" s="74"/>
-      <c r="T20" s="74"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="74"/>
-      <c r="W20" s="74"/>
-      <c r="X20" s="74"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
     </row>
     <row r="21" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D21" s="55">
@@ -3625,25 +3629,25 @@
       <c r="E21" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="74"/>
-      <c r="Q21" s="74"/>
-      <c r="R21" s="74"/>
-      <c r="S21" s="74"/>
-      <c r="T21" s="74"/>
-      <c r="U21" s="74"/>
-      <c r="V21" s="74"/>
-      <c r="W21" s="74"/>
-      <c r="X21" s="74"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="57"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="57"/>
+      <c r="V21" s="57"/>
+      <c r="W21" s="57"/>
+      <c r="X21" s="57"/>
     </row>
     <row r="22" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D22" s="55">
@@ -3652,25 +3656,25 @@
       <c r="E22" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="74"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-      <c r="S22" s="74"/>
-      <c r="T22" s="74"/>
-      <c r="U22" s="74"/>
-      <c r="V22" s="74"/>
-      <c r="W22" s="74"/>
-      <c r="X22" s="74"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="57"/>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="57"/>
+      <c r="S22" s="57"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
     </row>
     <row r="23" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D23" s="55">
@@ -3679,31 +3683,31 @@
       <c r="E23" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74" t="s">
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="N23" s="74" t="s">
+      <c r="N23" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="O23" s="74"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="74"/>
-      <c r="R23" s="74"/>
-      <c r="S23" s="74"/>
-      <c r="T23" s="74"/>
-      <c r="U23" s="74" t="s">
+      <c r="O23" s="57"/>
+      <c r="P23" s="57"/>
+      <c r="Q23" s="57"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="V23" s="74"/>
-      <c r="W23" s="74"/>
-      <c r="X23" s="74"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
     </row>
     <row r="24" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D24" s="55">
@@ -3712,27 +3716,27 @@
       <c r="E24" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="74"/>
-      <c r="L24" s="74"/>
-      <c r="M24" s="74"/>
-      <c r="N24" s="74"/>
-      <c r="O24" s="74"/>
-      <c r="P24" s="74"/>
-      <c r="Q24" s="74" t="s">
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="57"/>
+      <c r="Q24" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="R24" s="74"/>
-      <c r="S24" s="74"/>
-      <c r="T24" s="74"/>
-      <c r="U24" s="74"/>
-      <c r="V24" s="74"/>
-      <c r="W24" s="74"/>
-      <c r="X24" s="74"/>
+      <c r="R24" s="57"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="57"/>
     </row>
     <row r="25" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D25" s="55">
@@ -3741,27 +3745,27 @@
       <c r="E25" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="F25" s="74" t="s">
+      <c r="F25" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="74"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="74"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
-      <c r="S25" s="74"/>
-      <c r="T25" s="74"/>
-      <c r="U25" s="74"/>
-      <c r="V25" s="74"/>
-      <c r="W25" s="74"/>
-      <c r="X25" s="74"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="57"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
     </row>
     <row r="26" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D26" s="55">
@@ -3770,27 +3774,27 @@
       <c r="E26" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="74" t="s">
+      <c r="F26" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="G26" s="74"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="74"/>
-      <c r="K26" s="74"/>
-      <c r="L26" s="74"/>
-      <c r="M26" s="74"/>
-      <c r="N26" s="74"/>
-      <c r="O26" s="74"/>
-      <c r="P26" s="74"/>
-      <c r="Q26" s="74"/>
-      <c r="R26" s="74"/>
-      <c r="S26" s="74"/>
-      <c r="T26" s="74"/>
-      <c r="U26" s="74"/>
-      <c r="V26" s="74"/>
-      <c r="W26" s="74"/>
-      <c r="X26" s="74"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="57"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
     </row>
   </sheetData>
   <autoFilter ref="E9:X26"/>
@@ -3803,4 +3807,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E7:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>